<commit_message>
Update advies-tabblad automatisch vanuit voetbal_odds.xlsx
</commit_message>
<xml_diff>
--- a/data/Advies.xlsx
+++ b/data/Advies.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="advies" sheetId="1" r:id="rId1"/>
+    <sheet name="Advies" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
   <si>
     <t>Wedstrijd</t>
   </si>
@@ -58,115 +58,262 @@
     <t>Link 2</t>
   </si>
   <si>
-    <t>Bulgarije vs Spanje</t>
+    <t>Argentinië vs Venezuela</t>
   </si>
   <si>
     <t>Uruguay vs Peru</t>
   </si>
   <si>
-    <t>Slowakije vs Duitsland</t>
+    <t>Ierland vs Hongarije</t>
+  </si>
+  <si>
+    <t>Nederland vs Polen</t>
   </si>
   <si>
     <t>totaal aantal schoten</t>
   </si>
   <si>
-    <t>nikolay minkov</t>
+    <t>totaal aantal schoten op doel</t>
+  </si>
+  <si>
+    <t>venezuela</t>
   </si>
   <si>
     <t>andy polo</t>
   </si>
   <si>
-    <t>david hancko</t>
+    <t>wedstrijd</t>
+  </si>
+  <si>
+    <t>jan paul van hecke</t>
   </si>
   <si>
     <t>uruguay</t>
   </si>
   <si>
+    <t>ierland</t>
+  </si>
+  <si>
+    <t>meer dan 8.5</t>
+  </si>
+  <si>
+    <t>meer dan 7.5</t>
+  </si>
+  <si>
+    <t>meer dan 1.5</t>
+  </si>
+  <si>
+    <t>meer dan 6.5</t>
+  </si>
+  <si>
     <t>meer dan 0.5</t>
   </si>
   <si>
-    <t>meer dan 1.5</t>
-  </si>
-  <si>
     <t>meer dan 16.5</t>
   </si>
   <si>
-    <t>vbet</t>
+    <t>meer dan 2.5</t>
+  </si>
+  <si>
+    <t>meer dan 9.5</t>
+  </si>
+  <si>
+    <t>meer dan 3.5</t>
+  </si>
+  <si>
+    <t>bet365</t>
+  </si>
+  <si>
+    <t>onecasino</t>
+  </si>
+  <si>
+    <t>bingoal</t>
   </si>
   <si>
     <t>jacks</t>
   </si>
   <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>minder dan 8.5</t>
+  </si>
+  <si>
+    <t>minder dan 7.5</t>
+  </si>
+  <si>
+    <t>minder dan 1.5</t>
+  </si>
+  <si>
+    <t>minder dan 6.5</t>
+  </si>
+  <si>
     <t>minder dan 0.5</t>
   </si>
   <si>
-    <t>minder dan 1.5</t>
-  </si>
-  <si>
     <t>minder dan 16.5</t>
   </si>
   <si>
-    <t>bingoal</t>
+    <t>minder dan 2.5</t>
+  </si>
+  <si>
+    <t>minder dan 9.5</t>
+  </si>
+  <si>
+    <t>minder dan 3.5</t>
   </si>
   <si>
     <t>starcasino</t>
   </si>
   <si>
-    <t>1=32, 2=118</t>
+    <t>1=52, 2=98</t>
+  </si>
+  <si>
+    <t>1=71, 2=79</t>
   </si>
   <si>
     <t>1=31, 2=119</t>
   </si>
   <si>
+    <t>1=56, 2=94</t>
+  </si>
+  <si>
+    <t>1=89, 2=61</t>
+  </si>
+  <si>
     <t>1=84, 2=66</t>
   </si>
   <si>
-    <t>1=86, 2=64</t>
+    <t>1=77, 2=73</t>
   </si>
   <si>
     <t>1=61, 2=89</t>
   </si>
   <si>
-    <t>1=34, 2=116</t>
-  </si>
-  <si>
-    <t>€8.12</t>
+    <t>1=97, 2=53</t>
+  </si>
+  <si>
+    <t>1=82, 2=68</t>
+  </si>
+  <si>
+    <t>1=38, 2=112</t>
+  </si>
+  <si>
+    <t>1=51, 2=99</t>
+  </si>
+  <si>
+    <t>1=83, 2=67</t>
+  </si>
+  <si>
+    <t>€6.0</t>
+  </si>
+  <si>
+    <t>€5.63</t>
   </si>
   <si>
     <t>€4.7</t>
   </si>
   <si>
+    <t>€4.0</t>
+  </si>
+  <si>
+    <t>€3.73</t>
+  </si>
+  <si>
+    <t>€3.4</t>
+  </si>
+  <si>
     <t>€3.72</t>
   </si>
   <si>
-    <t>€3.6</t>
+    <t>€3.3</t>
   </si>
   <si>
     <t>€2.5</t>
   </si>
   <si>
-    <t>€3.0</t>
-  </si>
-  <si>
-    <t>https://www.vbet.nl/nl/sports/pre-match/event-view/Soccer/World/18277589/world-cup-europe-qualification/27465623/bulgarije-spanje</t>
-  </si>
-  <si>
-    <t>https://www.vbet.nl/nl/sports/pre-match/event-view/Soccer/World/18278053/wereldbeker-zuidamerika-kwalificatie/27835743/uruguay-peru</t>
-  </si>
-  <si>
-    <t>https://www.vbet.nl/nl/sports/pre-match/event-view/Soccer/World/18277589/world-cup-europe-qualification/27465621/slowakije-duitsland</t>
-  </si>
-  <si>
-    <t>https://www.jacks.nl/sports/event/1024296376</t>
-  </si>
-  <si>
-    <t>https://www.bingoal.nl/sports/#event=1023224903&amp;betoffer=2549354482&amp;outcome=3855184199</t>
-  </si>
-  <si>
-    <t>https://www.jacks.nl/sports/event/1023224851</t>
+    <t>€2.43</t>
+  </si>
+  <si>
+    <t>€1.7</t>
+  </si>
+  <si>
+    <t>€2.0</t>
+  </si>
+  <si>
+    <t>€1.8</t>
+  </si>
+  <si>
+    <t>€0.75</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=179824574-1534851354~2/1&amp;bet=1#/AC/B1/C1/D8/E179824574/F3/P1</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=179824574-1534851300~6/5&amp;bet=1#/AC/B1/C1/D8/E179824574/F3/P1</t>
+  </si>
+  <si>
+    <t>https://sports.onecasino.nl/#/event/9696212</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=178036253-1547672347~7/4&amp;bet=1#/AC/B1/C1/D8/E178036253/F3/P1</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=179824574-1534716251~8/11&amp;bet=1#/AC/B1/C1/D8/E179824574/F3/P1</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1023224937&amp;betoffer=2549012920&amp;outcome=3854248387</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=178036253-1547672330~1/1&amp;bet=1#/AC/B1/C1/D8/E178036253/F3/P1</t>
+  </si>
+  <si>
+    <t>https://jacks.nl/sports/event/1024296376#event/1024296376</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=178036253-1547948350~4/7&amp;bet=1#/AC/B1/C1/D8/E178036253/F3/P1</t>
+  </si>
+  <si>
+    <t>https://sport.toto.nl/wedden/wedstrijd/8660491</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=179824574-1534851304~3/1&amp;bet=1#/AC/B1/C1/D8/E179824574/F3/P1</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=178036253-1547672335~3/1&amp;bet=1#/AC/B1/C1/D8/E178036253/F3/P1</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=178036253-1547630556~5/6&amp;bet=1#/AC/B1/C1/D8/E178036253/F3/P1</t>
+  </si>
+  <si>
+    <t>https://jacks.nl/sports/event/1024296373#event/1024296373</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1022335882&amp;betoffer=2549604089&amp;outcome=3856371853</t>
+  </si>
+  <si>
+    <t>https://jacks.nl/sports/event/1023224937#event/1023224937</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1022335882&amp;betoffer=2549604112&amp;outcome=3856371919</t>
   </si>
   <si>
     <t>https://starcasino.nl/prematch-bets?page=event&amp;sportId=66&amp;eventId=13267842</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1022335882&amp;betoffer=2549604084&amp;outcome=3856371842</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=179824574-1534716244~5/4&amp;bet=1#/AC/B1/C1/D8/E179824574/F3/P1</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1022335882&amp;betoffer=2549604094&amp;outcome=3856371865</t>
+  </si>
+  <si>
+    <t>https://www.bet365.nl/?bs=179824574-1534850981~8/15&amp;bet=1#/AC/B1/C1/D8/E179824574/F3/P1</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1022335882&amp;betoffer=2549604197&amp;outcome=3856372161</t>
   </si>
 </sst>
 </file>
@@ -537,7 +684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -592,87 +739,87 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I2">
-        <v>1.34</v>
+        <v>1.6</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="L2">
-        <v>5.37</v>
+        <v>4.17</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>2.2</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="I3">
-        <v>1.3</v>
+        <v>1.97</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="L3">
-        <v>3.08</v>
+        <v>3.78</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -680,43 +827,43 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F4">
-        <v>1.83</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="I4">
-        <v>2.35</v>
+        <v>1.3</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="L4">
-        <v>2.8</v>
+        <v>3.08</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -724,147 +871,561 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F5">
-        <v>1.8</v>
+        <v>2.75</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="I5">
-        <v>2.4</v>
+        <v>1.65</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="L5">
-        <v>2.78</v>
+        <v>3.03</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>2.5</v>
+        <v>1.727272727272727</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I6">
-        <v>1.7334</v>
+        <v>2.55</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="L6">
-        <v>2.31</v>
+        <v>2.89</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7">
+        <v>2.95</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7">
+        <v>1.58</v>
+      </c>
+      <c r="J7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7">
+        <v>2.81</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8">
+        <v>1.83</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>2.35</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8">
+        <v>2.8</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9">
+        <v>2.1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9">
+        <v>2.38</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10">
+        <v>1.7334</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10">
+        <v>2.31</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11">
+        <v>1.571428571428571</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11">
+        <v>2.9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11">
+        <v>1.88</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>1.85</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12">
+        <v>2.25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12">
+        <v>1.5</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13">
+        <v>1.36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13">
+        <v>1.47</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14">
+        <v>1.36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14">
+        <v>1.47</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15">
+        <v>1.533333333333333</v>
+      </c>
+      <c r="J15" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" t="s">
+        <v>75</v>
+      </c>
+      <c r="L15">
+        <v>1.45</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="F7">
-        <v>4.5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7">
-        <v>1.32</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <v>1.833333333333333</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
         <v>37</v>
       </c>
-      <c r="K7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7">
-        <v>2.02</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>49</v>
+      <c r="I16">
+        <v>2.25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16">
+        <v>1.01</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="N2" r:id="rId2" location="event=1023224903&amp;betoffer=2549354482&amp;outcome=3855184199"/>
-    <hyperlink ref="M3" r:id="rId3"/>
-    <hyperlink ref="N3" r:id="rId4"/>
-    <hyperlink ref="M4" r:id="rId5"/>
-    <hyperlink ref="N4" r:id="rId6"/>
-    <hyperlink ref="M5" r:id="rId7"/>
-    <hyperlink ref="N5" r:id="rId8"/>
-    <hyperlink ref="M6" r:id="rId9"/>
-    <hyperlink ref="N6" r:id="rId10"/>
-    <hyperlink ref="M7" r:id="rId11"/>
-    <hyperlink ref="N7" r:id="rId12"/>
+    <hyperlink ref="M2" r:id="rId1" location="/AC/B1/C1/D8/E179824574/F3/P1"/>
+    <hyperlink ref="N2" r:id="rId2" location="event/1024296373"/>
+    <hyperlink ref="M3" r:id="rId3" location="/AC/B1/C1/D8/E179824574/F3/P1"/>
+    <hyperlink ref="N3" r:id="rId4" location="event/1024296373"/>
+    <hyperlink ref="M4" r:id="rId5" location="/event/9696212"/>
+    <hyperlink ref="N4" r:id="rId6" location="event/1024296376"/>
+    <hyperlink ref="M5" r:id="rId7" location="/AC/B1/C1/D8/E178036253/F3/P1"/>
+    <hyperlink ref="N5" r:id="rId8" location="event=1022335882&amp;betoffer=2549604089&amp;outcome=3856371853"/>
+    <hyperlink ref="M6" r:id="rId9" location="/AC/B1/C1/D8/E179824574/F3/P1"/>
+    <hyperlink ref="N6" r:id="rId10" location="event/1024296373"/>
+    <hyperlink ref="M7" r:id="rId11" location="event=1023224937&amp;betoffer=2549012920&amp;outcome=3854248387"/>
+    <hyperlink ref="N7" r:id="rId12" location="event/1023224937"/>
+    <hyperlink ref="M8" r:id="rId13" location="/event/9696212"/>
+    <hyperlink ref="N8" r:id="rId14" location="event/1024296376"/>
+    <hyperlink ref="M9" r:id="rId15" location="/AC/B1/C1/D8/E178036253/F3/P1"/>
+    <hyperlink ref="N9" r:id="rId16" location="event=1022335882&amp;betoffer=2549604112&amp;outcome=3856371919"/>
+    <hyperlink ref="M10" r:id="rId17" location="event/1024296376"/>
+    <hyperlink ref="N10" r:id="rId18"/>
+    <hyperlink ref="M11" r:id="rId19" location="/AC/B1/C1/D8/E178036253/F3/P1"/>
+    <hyperlink ref="N11" r:id="rId20" location="event=1022335882&amp;betoffer=2549604084&amp;outcome=3856371842"/>
+    <hyperlink ref="M12" r:id="rId21"/>
+    <hyperlink ref="N12" r:id="rId22" location="/AC/B1/C1/D8/E179824574/F3/P1"/>
+    <hyperlink ref="M13" r:id="rId23" location="/AC/B1/C1/D8/E179824574/F3/P1"/>
+    <hyperlink ref="N13" r:id="rId24" location="event/1024296373"/>
+    <hyperlink ref="M14" r:id="rId25" location="/AC/B1/C1/D8/E178036253/F3/P1"/>
+    <hyperlink ref="N14" r:id="rId26" location="event=1022335882&amp;betoffer=2549604094&amp;outcome=3856371865"/>
+    <hyperlink ref="M15" r:id="rId27"/>
+    <hyperlink ref="N15" r:id="rId28" location="/AC/B1/C1/D8/E179824574/F3/P1"/>
+    <hyperlink ref="M16" r:id="rId29" location="/AC/B1/C1/D8/E178036253/F3/P1"/>
+    <hyperlink ref="N16" r:id="rId30" location="event=1022335882&amp;betoffer=2549604197&amp;outcome=3856372161"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update advies-tabblad + timestamp in A1
</commit_message>
<xml_diff>
--- a/data/Advies.xlsx
+++ b/data/Advies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="89">
   <si>
     <t>Wedstrijd</t>
   </si>
@@ -58,12 +58,15 @@
     <t>Link 2</t>
   </si>
   <si>
-    <t>Laatst bijgewerkt: 2025-09-05 14:53:33</t>
+    <t>Laatst bijgewerkt: 2025-09-05 18:53:17</t>
   </si>
   <si>
     <t>Chicago Fire vs New England Revolution</t>
   </si>
   <si>
+    <t>Duitsland vs Noord-Ierland</t>
+  </si>
+  <si>
     <t>Montenegro vs Tsjechië</t>
   </si>
   <si>
@@ -76,12 +79,21 @@
     <t>totaal aantal schoten op doel</t>
   </si>
   <si>
+    <t>totaal aantal schoten</t>
+  </si>
+  <si>
     <t>wedstrijd</t>
   </si>
   <si>
+    <t>duitsland</t>
+  </si>
+  <si>
     <t>montenegro</t>
   </si>
   <si>
+    <t>kylian mbappé</t>
+  </si>
+  <si>
     <t>oekraïne</t>
   </si>
   <si>
@@ -91,21 +103,33 @@
     <t>meer dan 10.5</t>
   </si>
   <si>
+    <t>meer dan 7.5</t>
+  </si>
+  <si>
+    <t>meer dan 8.5</t>
+  </si>
+  <si>
     <t>meer dan 3.5</t>
   </si>
   <si>
+    <t>meer dan 6.5</t>
+  </si>
+  <si>
+    <t>meer dan 4.5</t>
+  </si>
+  <si>
     <t>meer dan 2.5</t>
   </si>
   <si>
-    <t>meer dan 8.5</t>
-  </si>
-  <si>
     <t>meer dan 9.5</t>
   </si>
   <si>
     <t>onecasino</t>
   </si>
   <si>
+    <t>bingoal</t>
+  </si>
+  <si>
     <t>jacks</t>
   </si>
   <si>
@@ -115,27 +139,51 @@
     <t>minder dan 10.5</t>
   </si>
   <si>
+    <t>minder dan 7.5</t>
+  </si>
+  <si>
+    <t>minder dan 8.5</t>
+  </si>
+  <si>
     <t>minder dan 3.5</t>
   </si>
   <si>
+    <t>minder dan 6.5</t>
+  </si>
+  <si>
+    <t>minder dan 4.5</t>
+  </si>
+  <si>
     <t>minder dan 2.5</t>
   </si>
   <si>
-    <t>minder dan 8.5</t>
-  </si>
-  <si>
     <t>minder dan 9.5</t>
   </si>
   <si>
     <t>starcasino</t>
   </si>
   <si>
-    <t>1=58, 2=92</t>
+    <t>1=59, 2=91</t>
+  </si>
+  <si>
+    <t>1=75, 2=75</t>
+  </si>
+  <si>
+    <t>1=55, 2=95</t>
   </si>
   <si>
     <t>1=60, 2=90</t>
   </si>
   <si>
+    <t>1=96, 2=54</t>
+  </si>
+  <si>
+    <t>1=61, 2=89</t>
+  </si>
+  <si>
+    <t>1=74, 2=76</t>
+  </si>
+  <si>
     <t>1=44, 2=106</t>
   </si>
   <si>
@@ -145,18 +193,27 @@
     <t>1=93, 2=57</t>
   </si>
   <si>
-    <t>1=74, 2=76</t>
-  </si>
-  <si>
-    <t>1=55, 2=95</t>
-  </si>
-  <si>
-    <t>€8.92</t>
+    <t>€9.25</t>
+  </si>
+  <si>
+    <t>€6.0</t>
+  </si>
+  <si>
+    <t>€5.8</t>
   </si>
   <si>
     <t>€5.46</t>
   </si>
   <si>
+    <t>€4.56</t>
+  </si>
+  <si>
+    <t>€3.73</t>
+  </si>
+  <si>
+    <t>€3.52</t>
+  </si>
+  <si>
     <t>€3.12</t>
   </si>
   <si>
@@ -169,31 +226,61 @@
     <t>€1.7</t>
   </si>
   <si>
+    <t>€1.3</t>
+  </si>
+  <si>
     <t>€1.25</t>
   </si>
   <si>
     <t>https://sports.onecasino.nl/#/event/10025497</t>
   </si>
   <si>
+    <t>https://www.bingoal.nl/sports/#event=1023224852&amp;betoffer=2552162167&amp;outcome=3865656359</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1023224852&amp;betoffer=2552162170&amp;outcome=3865656366</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1023168639&amp;betoffer=2549626618&amp;outcome=3856355987</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1023224852&amp;betoffer=2552162169&amp;outcome=3865656364</t>
+  </si>
+  <si>
     <t>https://jacks.nl/sports/event/1023168639#event/1023168639</t>
   </si>
   <si>
     <t>https://sport.toto.nl/wedden/wedstrijd/8590797</t>
   </si>
   <si>
-    <t>https://jacks.nl/sports/event/1022335870#event/1022335870</t>
+    <t>https://www.bingoal.nl/sports/#event=1022335870&amp;betoffer=2549614664&amp;outcome=3856406727</t>
+  </si>
+  <si>
+    <t>https://www.bingoal.nl/sports/#event=1023168639&amp;betoffer=2549626614&amp;outcome=3856355980</t>
+  </si>
+  <si>
+    <t>https://sport.toto.nl/wedden/wedstrijd/8778584</t>
   </si>
   <si>
     <t>https://starcasino.nl/prematch-bets?page=event&amp;sportId=66&amp;eventId=11998073</t>
   </si>
   <si>
+    <t>https://jacks.nl/sports/event/1023224852#event/1023224852</t>
+  </si>
+  <si>
     <t>https://starcasino.nl/prematch-bets?page=event&amp;sportId=66&amp;eventId=13549442</t>
   </si>
   <si>
+    <t>https://jacks.nl/sports/event/1023224887#event/1023224887</t>
+  </si>
+  <si>
     <t>https://starcasino.nl/prematch-bets?page=event&amp;sportId=66&amp;eventId=12623890</t>
   </si>
   <si>
     <t>https://starcasino.nl/prematch-bets?page=event&amp;sportId=66&amp;eventId=12623891</t>
+  </si>
+  <si>
+    <t>https://sports.onecasino.nl/#/event/10028349</t>
   </si>
 </sst>
 </file>
@@ -564,7 +651,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,43 +711,43 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F3">
-        <v>2.74</v>
+        <v>2.73</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I3">
         <v>1.75</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="L3">
-        <v>6.36</v>
+        <v>6.23</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -668,131 +755,131 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F4">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4">
-        <v>1.7273</v>
+        <v>2.08</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="L4">
-        <v>3.64</v>
+        <v>4.3</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F5">
-        <v>3.5</v>
+        <v>2.85</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I5">
-        <v>1.4445</v>
+        <v>1.64</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="L5">
-        <v>2.2</v>
+        <v>3.94</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F6">
-        <v>2.33</v>
+        <v>2.6</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I6">
-        <v>1.8182</v>
+        <v>1.7273</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="L6">
-        <v>2.08</v>
+        <v>3.64</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -800,43 +887,43 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F7">
-        <v>1.65</v>
+        <v>1.61</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I7">
-        <v>2.6667</v>
+        <v>2.88</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="L7">
-        <v>1.89</v>
+        <v>3.17</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -844,151 +931,473 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F8">
-        <v>2.05</v>
+        <v>2.55</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1.7273</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="L8">
-        <v>1.22</v>
+        <v>2.89</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F9">
-        <v>2.05</v>
+        <v>2.09</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="K9" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="L9">
-        <v>1.22</v>
+        <v>2.65</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10">
+        <v>3.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10">
+        <v>1.4445</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10">
+        <v>2.2</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11">
+        <v>2.33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11">
+        <v>1.8182</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11">
+        <v>2.08</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12">
+        <v>1.65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12">
+        <v>2.6667</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12">
+        <v>1.89</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13">
+        <v>1.64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13">
+        <v>2.6667</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13">
+        <v>1.52</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14">
+        <v>2.05</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14">
+        <v>1.22</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15">
+        <v>2.05</v>
+      </c>
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15">
+        <v>1.22</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10">
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16">
+        <v>2.5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16">
+        <v>1.7</v>
+      </c>
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" t="s">
+        <v>70</v>
+      </c>
+      <c r="L16">
+        <v>1.18</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17">
         <v>2.75</v>
       </c>
-      <c r="G10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10">
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17">
         <v>1.6</v>
       </c>
-      <c r="J10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="J17" t="s">
         <v>51</v>
       </c>
-      <c r="L10">
+      <c r="K17" t="s">
+        <v>71</v>
+      </c>
+      <c r="L17">
         <v>1.14</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>58</v>
+      <c r="M17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M3" r:id="rId1" location="/event/10025497"/>
     <hyperlink ref="N3" r:id="rId2"/>
-    <hyperlink ref="M4" r:id="rId3" location="event/1023168639"/>
-    <hyperlink ref="N4" r:id="rId4"/>
-    <hyperlink ref="M5" r:id="rId5"/>
-    <hyperlink ref="N5" r:id="rId6"/>
-    <hyperlink ref="M6" r:id="rId7" location="event/1022335870"/>
+    <hyperlink ref="M4" r:id="rId3" location="event=1023224852&amp;betoffer=2552162167&amp;outcome=3865656359"/>
+    <hyperlink ref="N4" r:id="rId4" location="event/1023224852"/>
+    <hyperlink ref="M5" r:id="rId5" location="event=1023224852&amp;betoffer=2552162170&amp;outcome=3865656366"/>
+    <hyperlink ref="N5" r:id="rId6" location="event/1023224852"/>
+    <hyperlink ref="M6" r:id="rId7" location="event=1023168639&amp;betoffer=2549626618&amp;outcome=3856355987"/>
     <hyperlink ref="N6" r:id="rId8"/>
-    <hyperlink ref="M7" r:id="rId9" location="event/1023168639"/>
-    <hyperlink ref="N7" r:id="rId10"/>
-    <hyperlink ref="M8" r:id="rId11"/>
+    <hyperlink ref="M7" r:id="rId9" location="event=1023224852&amp;betoffer=2552162169&amp;outcome=3865656364"/>
+    <hyperlink ref="N7" r:id="rId10" location="event/1023224852"/>
+    <hyperlink ref="M8" r:id="rId11" location="event/1023168639"/>
     <hyperlink ref="N8" r:id="rId12"/>
     <hyperlink ref="M9" r:id="rId13"/>
-    <hyperlink ref="N9" r:id="rId14"/>
+    <hyperlink ref="N9" r:id="rId14" location="event/1023224887"/>
     <hyperlink ref="M10" r:id="rId15"/>
     <hyperlink ref="N10" r:id="rId16"/>
+    <hyperlink ref="M11" r:id="rId17" location="event=1022335870&amp;betoffer=2549614664&amp;outcome=3856406727"/>
+    <hyperlink ref="N11" r:id="rId18"/>
+    <hyperlink ref="M12" r:id="rId19" location="event=1023168639&amp;betoffer=2549626614&amp;outcome=3856355980"/>
+    <hyperlink ref="N12" r:id="rId20"/>
+    <hyperlink ref="M13" r:id="rId21" location="event/1023168639"/>
+    <hyperlink ref="N13" r:id="rId22"/>
+    <hyperlink ref="M14" r:id="rId23"/>
+    <hyperlink ref="N14" r:id="rId24"/>
+    <hyperlink ref="M15" r:id="rId25"/>
+    <hyperlink ref="N15" r:id="rId26"/>
+    <hyperlink ref="M16" r:id="rId27"/>
+    <hyperlink ref="N16" r:id="rId28" location="/event/10028349"/>
+    <hyperlink ref="M17" r:id="rId29"/>
+    <hyperlink ref="N17" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>